<commit_message>
purge more pytz calls, fix test parser header
</commit_message>
<xml_diff>
--- a/bio_diversity/static/test/parser_test_files/test-water_quality_record.xlsx
+++ b/bio_diversity/static/test/parser_test_files/test-water_quality_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyelq\Desktop\Work\dm_apps\dm_apps\bio_diversity\static\test\parser_test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B999251-6344-4661-B6DF-7C7F5AAFA3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCEAF6A-23AC-4071-A928-02F5EA7C86A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="270" windowWidth="24720" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Water Quality Data" sheetId="6" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Fish in Pond?</t>
   </si>
   <si>
-    <t>Time (24HR)</t>
-  </si>
-  <si>
     <t>SP3</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -452,16 +454,16 @@
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
@@ -482,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>5</v>
@@ -496,20 +498,20 @@
         <v>2021</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
       </c>
       <c r="I4">
         <v>89.6</v>
@@ -521,7 +523,7 @@
         <v>101</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -529,20 +531,20 @@
         <v>2021</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5">
         <v>13.5</v>
@@ -554,7 +556,7 @@
         <v>105</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>